<commit_message>
New data for time.clock()
</commit_message>
<xml_diff>
--- a/Project1.xlsx
+++ b/Project1.xlsx
@@ -71,7 +71,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -213,9 +214,6 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:v>Run2</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
               <a:noFill/>
@@ -248,14 +246,14 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="power"/>
+            <c:trendlineType val="exp"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-5.2063429571303589E-2"/>
-                  <c:y val="-8.8419364246135945E-2"/>
+                  <c:x val="3.3211723534558181E-2"/>
+                  <c:y val="6.2198891805191017E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -290,10 +288,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$14</c:f>
+              <c:f>Sheet1!$A$2:$A$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>4</c:v>
                 </c:pt>
@@ -338,30 +336,30 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$14</c:f>
+              <c:f>Sheet1!$B$2:$B$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>105</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1002</c:v>
+                  <c:v>322</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1003</c:v>
+                  <c:v>942</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2993</c:v>
+                  <c:v>2863</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9026</c:v>
+                  <c:v>8730</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>27064</c:v>
+                  <c:v>24690</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>73170</c:v>
@@ -2696,10 +2694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2707,7 +2705,7 @@
     <col min="2" max="2" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2721,12 +2719,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>4</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="C2">
         <v>0.70709999999999995</v>
@@ -2735,12 +2733,12 @@
         <v>0.88959999999999995</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>5</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>105</v>
       </c>
       <c r="C3">
         <v>0.89439999999999997</v>
@@ -2749,12 +2747,12 @@
         <v>1.0654999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>6</v>
       </c>
       <c r="B4">
-        <v>1002</v>
+        <v>322</v>
       </c>
       <c r="C4">
         <v>0.95740000000000003</v>
@@ -2763,12 +2761,12 @@
         <v>1.2210000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>7</v>
       </c>
       <c r="B5">
-        <v>1003</v>
+        <v>942</v>
       </c>
       <c r="C5">
         <v>1.03</v>
@@ -2777,12 +2775,12 @@
         <v>1.3779999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>8</v>
       </c>
       <c r="B6">
-        <v>2993</v>
+        <v>2863</v>
       </c>
       <c r="C6">
         <v>1.1040000000000001</v>
@@ -2791,12 +2789,12 @@
         <v>1.52</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>9</v>
       </c>
       <c r="B7">
-        <v>9026</v>
+        <v>8730</v>
       </c>
       <c r="C7">
         <v>1.155</v>
@@ -2805,12 +2803,12 @@
         <v>1.6659999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>10</v>
       </c>
       <c r="B8">
-        <v>27064</v>
+        <v>24690</v>
       </c>
       <c r="C8">
         <v>1.2689999999999999</v>
@@ -2819,11 +2817,11 @@
         <v>1.8009999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>11</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>73170</v>
       </c>
       <c r="C9">
@@ -2832,12 +2830,13 @@
       <c r="D9">
         <v>1.9379999999999999</v>
       </c>
+      <c r="Q9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>12</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>207552</v>
       </c>
       <c r="C10">
@@ -2846,12 +2845,13 @@
       <c r="D10">
         <v>2.0670000000000002</v>
       </c>
+      <c r="Q10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>13</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>592576</v>
       </c>
       <c r="C11">
@@ -2860,12 +2860,13 @@
       <c r="D11">
         <v>2.198</v>
       </c>
+      <c r="Q11" s="1"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>14</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>1797750</v>
       </c>
       <c r="C12">
@@ -2874,12 +2875,13 @@
       <c r="D12">
         <v>2.323</v>
       </c>
+      <c r="Q12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>15</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <v>5098584</v>
       </c>
       <c r="C13">
@@ -2888,12 +2890,13 @@
       <c r="D13">
         <v>2.448</v>
       </c>
+      <c r="Q13" s="1"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>16</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <v>14769302</v>
       </c>
       <c r="C14">
@@ -2902,9 +2905,32 @@
       <c r="D14">
         <v>2.569</v>
       </c>
+      <c r="Q14" s="1"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="Q15" s="1"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="Q16" s="1"/>
+    </row>
+    <row r="17" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q17" s="1"/>
+    </row>
+    <row r="18" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q18" s="1"/>
+    </row>
+    <row r="19" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q19" s="1"/>
+    </row>
+    <row r="20" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q20" s="1"/>
+    </row>
+    <row r="21" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q21" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>